<commit_message>
Updated plan and day 2 presentation on AI
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0231331C-35A1-4E65-A379-D89FFE14D5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94179091-81ED-474D-834B-435A1EE61D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -678,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -789,6 +789,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -799,9 +802,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFB871"/>
       <color rgb="FFAFFFAB"/>
       <color rgb="FFFFEE6D"/>
-      <color rgb="FFFFB871"/>
       <color rgb="FFFF9393"/>
     </mruColors>
   </colors>
@@ -1323,7 +1326,7 @@
   <dimension ref="C3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,7 +1419,7 @@
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="38" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
@@ -1565,12 +1568,12 @@
     <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added info to day 2 presentation
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94179091-81ED-474D-834B-435A1EE61D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62B6DFC-0F64-4CBC-85E2-80079BECAA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
   <si>
     <t>lesson 1</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t xml:space="preserve">Первый ии - советник императора </t>
+  </si>
+  <si>
+    <t>Код Цезаря - шифровка и расшифровка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Задания на перевод </t>
   </si>
 </sst>
 </file>
@@ -761,6 +767,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -773,6 +782,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -783,15 +798,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -803,8 +809,8 @@
   <colors>
     <mruColors>
       <color rgb="FFFFB871"/>
+      <color rgb="FFFFEE6D"/>
       <color rgb="FFAFFFAB"/>
-      <color rgb="FFFFEE6D"/>
       <color rgb="FFFF9393"/>
     </mruColors>
   </colors>
@@ -1282,10 +1288,10 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="26" t="s">
         <v>41</v>
       </c>
@@ -1296,8 +1302,8 @@
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="29"/>
-      <c r="D15" s="31"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="15" t="s">
         <v>42</v>
       </c>
@@ -1326,7 +1332,7 @@
   <dimension ref="C3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1370,9 @@
       <c r="D5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="F5" s="13" t="s">
         <v>20</v>
       </c>
@@ -1402,7 +1410,9 @@
       <c r="D7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="13" t="s">
+        <v>62</v>
+      </c>
       <c r="F7" s="13" t="s">
         <v>37</v>
       </c>
@@ -1419,7 +1429,7 @@
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="28" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
@@ -1436,20 +1446,20 @@
       </c>
     </row>
     <row r="9" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="37" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="36"/>
+      <c r="H9" s="33"/>
       <c r="L9" s="22" t="s">
         <v>24</v>
       </c>
@@ -1458,14 +1468,14 @@
       </c>
     </row>
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="33"/>
-      <c r="D10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="35"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="37"/>
+      <c r="H10" s="34"/>
       <c r="L10" s="20" t="s">
         <v>38</v>
       </c>
@@ -1538,10 +1548,10 @@
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="30"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="26" t="s">
         <v>41</v>
       </c>
@@ -1552,8 +1562,8 @@
       <c r="H15" s="25"/>
     </row>
     <row r="16" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="29"/>
-      <c r="D16" s="31"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="15" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Added info to day 3 AI presentation
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E46CD4-288C-425D-A057-29002D4FDDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5C6ACD-19C3-4547-A705-EA4FF2EEF135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -684,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -767,6 +767,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -797,7 +800,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -808,8 +811,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFB871"/>
       <color rgb="FFFFEE6D"/>
-      <color rgb="FFFFB871"/>
       <color rgb="FFAFFFAB"/>
       <color rgb="FFFF9393"/>
     </mruColors>
@@ -1090,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1188,7 @@
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="28" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
@@ -1225,7 +1228,7 @@
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="39" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="15" t="s">
@@ -1288,10 +1291,10 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="26" t="s">
         <v>41</v>
       </c>
@@ -1302,8 +1305,8 @@
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="29"/>
-      <c r="D15" s="31"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="15" t="s">
         <v>42</v>
       </c>
@@ -1332,7 +1335,7 @@
   <dimension ref="C3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="L13" sqref="L12:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1432,7 @@
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="28" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
@@ -1446,20 +1449,20 @@
       </c>
     </row>
     <row r="9" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="37" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="32"/>
+      <c r="H9" s="33"/>
       <c r="L9" s="22" t="s">
         <v>24</v>
       </c>
@@ -1468,14 +1471,14 @@
       </c>
     </row>
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="35"/>
-      <c r="D10" s="37"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="37"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="33"/>
+      <c r="H10" s="34"/>
       <c r="L10" s="20" t="s">
         <v>38</v>
       </c>
@@ -1487,7 +1490,7 @@
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="39" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="15" t="s">
@@ -1548,10 +1551,10 @@
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="30"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="26" t="s">
         <v>41</v>
       </c>
@@ -1562,8 +1565,8 @@
       <c r="H15" s="25"/>
     </row>
     <row r="16" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="29"/>
-      <c r="D16" s="31"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="15" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Changed plan.xlsx 1 th and 2 th day
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5C6ACD-19C3-4547-A705-EA4FF2EEF135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB38A6-6E12-4508-9529-FC4B8FEB5E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
   <si>
     <t>lesson 1</t>
   </si>
@@ -258,17 +258,75 @@
     <t xml:space="preserve">Первый ии - советник императора </t>
   </si>
   <si>
-    <t>Код Цезаря - шифровка и расшифровка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Задания на перевод </t>
+    <r>
+      <t xml:space="preserve">Что такое ИТ, задумка лагеря - тема </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Питон введение</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Код Цезаря - шифровка и расшифровка</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Вывод + математика </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Бинарный код, unicode, ASCII, интернет </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Питон базовые типы данных + input (если успеваем)</t>
+    </r>
+  </si>
+  <si>
+    <t>Задания по типам данных + input</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +365,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,6 +405,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -684,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -770,6 +842,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -800,7 +875,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1228,7 +1306,7 @@
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="29" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="15" t="s">
@@ -1291,10 +1369,10 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="31"/>
+      <c r="D14" s="32"/>
       <c r="E14" s="26" t="s">
         <v>41</v>
       </c>
@@ -1305,8 +1383,8 @@
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="30"/>
-      <c r="D15" s="32"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="15" t="s">
         <v>42</v>
       </c>
@@ -1335,7 +1413,7 @@
   <dimension ref="C3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L13" sqref="L12:L13"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,13 +1448,13 @@
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>19</v>
+      <c r="D5" s="40" t="s">
+        <v>61</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="41" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="13"/>
@@ -1411,15 +1489,15 @@
         <v>7</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="41" t="s">
         <v>49</v>
       </c>
       <c r="H7" s="14"/>
@@ -1449,20 +1527,20 @@
       </c>
     </row>
     <row r="9" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="38" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="37"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="33"/>
+      <c r="H9" s="34"/>
       <c r="L9" s="22" t="s">
         <v>24</v>
       </c>
@@ -1471,14 +1549,14 @@
       </c>
     </row>
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="36"/>
-      <c r="D10" s="38"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="39"/>
       <c r="E10" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="38"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="34"/>
+      <c r="H10" s="35"/>
       <c r="L10" s="20" t="s">
         <v>38</v>
       </c>
@@ -1490,7 +1568,7 @@
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="29" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="15" t="s">
@@ -1551,10 +1629,10 @@
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="31"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="26" t="s">
         <v>41</v>
       </c>
@@ -1565,8 +1643,8 @@
       <c r="H15" s="25"/>
     </row>
     <row r="16" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="30"/>
-      <c r="D16" s="32"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="33"/>
       <c r="E16" s="15" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Addet day 1 and day 2 presentations about python, also added day 1 tasks
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB38A6-6E12-4508-9529-FC4B8FEB5E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A283C750-B697-462D-9B81-0382059FEA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
   <si>
     <t>lesson 1</t>
   </si>
@@ -258,75 +258,26 @@
     <t xml:space="preserve">Первый ии - советник императора </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Что такое ИТ, задумка лагеря - тема </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Питон введение</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Код Цезаря - шифровка и расшифровка</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Вывод + математика </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Бинарный код, unicode, ASCII, интернет </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Питон базовые типы данных + input (если успеваем)</t>
-    </r>
-  </si>
-  <si>
-    <t>Задания по типам данных + input</t>
+    <t>Питон введение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вывод + математика </t>
+  </si>
+  <si>
+    <t>Питон базовые типы данных + переменные + input (если успеваем)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Задания по типам данных + input + f-строки </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Задания </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,14 +310,6 @@
     <font>
       <b/>
       <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -875,10 +818,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -889,10 +832,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9393"/>
+      <color rgb="FFAFFFAB"/>
       <color rgb="FFFFB871"/>
       <color rgb="FFFFEE6D"/>
-      <color rgb="FFAFFFAB"/>
-      <color rgb="FFFF9393"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1413,7 +1356,7 @@
   <dimension ref="C3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,16 +1391,18 @@
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="41" t="s">
         <v>61</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="H5" s="14"/>
       <c r="L5" s="4"/>
       <c r="M5" s="5" t="s">
@@ -1494,11 +1439,9 @@
       <c r="E7" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>49</v>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="H7" s="14"/>
       <c r="L7" s="8"/>

</xml_diff>

<commit_message>
Added tasks.py to day 2
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3F841F-6487-44DC-B88C-876B5F8AC9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B06CBB-E742-48DB-9B39-098B4523772B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1356,7 +1356,7 @@
   <dimension ref="C3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added game 'Spiegs' rules and answer - questions
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B06CBB-E742-48DB-9B39-098B4523772B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49DD289-C878-4917-86D0-2D70263F26B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -822,6 +822,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -833,8 +836,8 @@
   <colors>
     <mruColors>
       <color rgb="FFAFFFAB"/>
+      <color rgb="FFFFB871"/>
       <color rgb="FFFF9393"/>
-      <color rgb="FFFFB871"/>
       <color rgb="FFFFEE6D"/>
     </mruColors>
   </colors>
@@ -1115,7 +1118,7 @@
   <dimension ref="C3:M16"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1158,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="30" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="13"/>
@@ -1193,10 +1196,10 @@
         <v>23</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="30" t="s">
         <v>49</v>
       </c>
       <c r="H7" s="14"/>
@@ -1213,7 +1216,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="29" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="15" t="s">
@@ -1356,7 +1359,7 @@
   <dimension ref="C3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,11 +1439,11 @@
       <c r="D7" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="31" t="s">
         <v>64</v>
       </c>
       <c r="F7" s="13"/>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="31" t="s">
         <v>65</v>
       </c>
       <c r="H7" s="14"/>
@@ -1457,7 +1460,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="42" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="15" t="s">

</xml_diff>

<commit_message>
Added day 3 presentation about language comparison
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49DD289-C878-4917-86D0-2D70263F26B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C694A-2991-4E7A-A964-3C741892D239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>lesson 1</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Презентация о unity и подводка к заданию - надо представить как будет выглядеть  город в будущем</t>
   </si>
   <si>
-    <t>Сравнение языков + подводка к созданию сайта как у больших ИТ компаний + немного GIT</t>
-  </si>
-  <si>
     <t>Исправляют баг в коде с комментариями + github</t>
   </si>
   <si>
@@ -271,6 +268,15 @@
   </si>
   <si>
     <t xml:space="preserve">Задания </t>
+  </si>
+  <si>
+    <t>Сравнение языков</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Подводка к созданию сайта как у больших ИТ компаний + немного GIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
@@ -1305,7 +1311,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>36</v>
@@ -1359,7 +1365,7 @@
   <dimension ref="C3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,16 +1401,16 @@
         <v>0</v>
       </c>
       <c r="D5" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>61</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>62</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H5" s="14"/>
       <c r="L5" s="4"/>
@@ -1437,14 +1443,14 @@
         <v>7</v>
       </c>
       <c r="D7" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="31" t="s">
         <v>63</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>64</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7" s="14"/>
       <c r="L7" s="8"/>
@@ -1476,8 +1482,8 @@
       <c r="C9" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="40" t="s">
-        <v>55</v>
+      <c r="D9" s="31" t="s">
+        <v>65</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>51</v>
@@ -1496,7 +1502,9 @@
     </row>
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="39"/>
-      <c r="D10" s="41"/>
+      <c r="D10" s="26" t="s">
+        <v>66</v>
+      </c>
       <c r="E10" s="26" t="s">
         <v>28</v>
       </c>
@@ -1525,6 +1533,9 @@
         <v>46</v>
       </c>
       <c r="H11" s="16"/>
+      <c r="M11" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
@@ -1563,14 +1574,14 @@
         <v>13</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -1604,12 +1615,11 @@
     </row>
     <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
     <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added day 3 presentation about HTML + CSS
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C694A-2991-4E7A-A964-3C741892D239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BAE755-75FC-4418-AF99-145F9C6CF4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -701,11 +701,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -800,6 +811,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -830,7 +847,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -841,9 +873,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9393"/>
       <color rgb="FFAFFFAB"/>
       <color rgb="FFFFB871"/>
-      <color rgb="FFFF9393"/>
       <color rgb="FFFFEE6D"/>
     </mruColors>
   </colors>
@@ -1321,10 +1353,10 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="26" t="s">
         <v>41</v>
       </c>
@@ -1335,8 +1367,8 @@
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="33"/>
-      <c r="D15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="15" t="s">
         <v>42</v>
       </c>
@@ -1362,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53492BD-B09C-4A09-8913-63C13D46C685}">
-  <dimension ref="C3:M17"/>
+  <dimension ref="C3:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,7 +1498,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="33" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="15" t="s">
@@ -1479,7 +1511,7 @@
       </c>
     </row>
     <row r="9" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="40" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="31" t="s">
@@ -1488,11 +1520,11 @@
       <c r="E9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="36"/>
+      <c r="H9" s="38"/>
       <c r="L9" s="22" t="s">
         <v>24</v>
       </c>
@@ -1501,16 +1533,16 @@
       </c>
     </row>
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="39"/>
-      <c r="D10" s="26" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="44" t="s">
         <v>66</v>
       </c>
       <c r="E10" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="37"/>
+      <c r="H10" s="39"/>
       <c r="L10" s="20" t="s">
         <v>38</v>
       </c>
@@ -1518,109 +1550,120 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="3:13" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="3" t="s">
+    <row r="11" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="45"/>
+      <c r="D11" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="25"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="47"/>
+    </row>
+    <row r="12" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="15" t="s">
+      <c r="D12" s="49"/>
+      <c r="E12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15" t="s">
+      <c r="F12" s="15"/>
+      <c r="G12" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="M11" s="1" t="s">
+      <c r="H12" s="16"/>
+      <c r="M12" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
+    <row r="13" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E13" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13" t="s">
+      <c r="F13" s="13"/>
+      <c r="G13" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="3" t="s">
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15" t="s">
+      <c r="E14" s="15"/>
+      <c r="F14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="12" t="s">
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D15" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E15" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17" t="s">
+      <c r="F15" s="17"/>
+      <c r="G15" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="32" t="s">
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="26" t="s">
+      <c r="D16" s="36"/>
+      <c r="E16" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24" t="s">
+      <c r="F16" s="24"/>
+      <c r="G16" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="33"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="15" t="s">
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="3:8" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="35"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G17" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="16"/>
-    </row>
-    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="F9:F10"/>
+    <mergeCell ref="D11:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GitLab + VietnesHosting presentation for day 3
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BAE755-75FC-4418-AF99-145F9C6CF4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650DBF0E-D8B8-44AC-B7DF-F3C62298D338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
   <si>
     <t>lesson 1</t>
   </si>
@@ -225,12 +225,6 @@
     <t xml:space="preserve">Kahoot игра </t>
   </si>
   <si>
-    <t>аккаунты гугл</t>
-  </si>
-  <si>
-    <t>gitlab pages</t>
-  </si>
-  <si>
     <t>Создание города в unity с моделками из assets store</t>
   </si>
   <si>
@@ -277,13 +271,22 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Практика по презентации </t>
+  </si>
+  <si>
+    <t xml:space="preserve">темы про  которые будут сайты детей </t>
+  </si>
+  <si>
+    <t>Создания сайта с помощью нейросети, neocities.org</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +319,14 @@
     <font>
       <b/>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -716,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -814,6 +825,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -832,9 +849,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -844,25 +858,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -873,10 +899,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFF9393"/>
       <color rgb="FFAFFFAB"/>
       <color rgb="FFFFB871"/>
       <color rgb="FFFFEE6D"/>
+      <color rgb="FFFF9393"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1155,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:M16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
@@ -1343,7 +1369,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>36</v>
@@ -1353,10 +1379,10 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="26" t="s">
         <v>41</v>
       </c>
@@ -1367,8 +1393,8 @@
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="35"/>
-      <c r="D15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="39"/>
       <c r="E15" s="15" t="s">
         <v>42</v>
       </c>
@@ -1396,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53492BD-B09C-4A09-8913-63C13D46C685}">
   <dimension ref="C3:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,16 +1459,16 @@
         <v>0</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H5" s="14"/>
       <c r="L5" s="4"/>
@@ -1475,14 +1501,14 @@
         <v>7</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H7" s="14"/>
       <c r="L7" s="8"/>
@@ -1498,7 +1524,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="35" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="15" t="s">
@@ -1511,20 +1537,16 @@
       </c>
     </row>
     <row r="9" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="38"/>
+        <v>63</v>
+      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="40"/>
       <c r="L9" s="22" t="s">
         <v>24</v>
       </c>
@@ -1533,16 +1555,16 @@
       </c>
     </row>
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="41"/>
-      <c r="D10" s="44" t="s">
+      <c r="C10" s="42"/>
+      <c r="D10" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="39"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="52"/>
       <c r="L10" s="20" t="s">
         <v>38</v>
       </c>
@@ -1551,14 +1573,18 @@
       </c>
     </row>
     <row r="11" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="45"/>
-      <c r="D11" s="48" t="s">
+      <c r="C11" s="44"/>
+      <c r="D11" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="25"/>
+      <c r="E11" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="34"/>
+      <c r="G11" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="33"/>
       <c r="L11" s="46"/>
       <c r="M11" s="47"/>
     </row>
@@ -1566,7 +1592,7 @@
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="49"/>
+      <c r="D12" s="48"/>
       <c r="E12" s="15" t="s">
         <v>30</v>
       </c>
@@ -1576,24 +1602,24 @@
       </c>
       <c r="H12" s="16"/>
       <c r="M12" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="14"/>
+      <c r="E13" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
@@ -1616,22 +1642,22 @@
         <v>13</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="26" t="s">
         <v>41</v>
       </c>
@@ -1642,8 +1668,8 @@
       <c r="H16" s="25"/>
     </row>
     <row r="17" spans="3:8" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="35"/>
-      <c r="D17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="15" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Added day 3 AI presentation
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650DBF0E-D8B8-44AC-B7DF-F3C62298D338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437357B8-5324-484A-A97D-CED880DF23DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
   <si>
     <t>lesson 1</t>
   </si>
@@ -834,6 +834,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -849,6 +867,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -858,37 +879,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -899,8 +899,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFB871"/>
       <color rgb="FFAFFFAB"/>
-      <color rgb="FFFFB871"/>
       <color rgb="FFFFEE6D"/>
       <color rgb="FFFF9393"/>
     </mruColors>
@@ -1182,7 +1182,7 @@
   <dimension ref="C3:M16"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1296,7 @@
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="54" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="13" t="s">
@@ -1316,7 +1316,7 @@
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="35" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="15" t="s">
@@ -1379,10 +1379,10 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="38"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="26" t="s">
         <v>41</v>
       </c>
@@ -1393,8 +1393,8 @@
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="37"/>
-      <c r="D15" s="39"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="15" t="s">
         <v>42</v>
       </c>
@@ -1422,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53492BD-B09C-4A09-8913-63C13D46C685}">
   <dimension ref="C3:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,9 +1464,7 @@
       <c r="E5" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="30" t="s">
-        <v>20</v>
-      </c>
+      <c r="F5" s="13"/>
       <c r="G5" s="31" t="s">
         <v>62</v>
       </c>
@@ -1537,16 +1535,16 @@
       </c>
     </row>
     <row r="9" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="48" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="49"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="46"/>
       <c r="L9" s="22" t="s">
         <v>24</v>
       </c>
@@ -1555,16 +1553,16 @@
       </c>
     </row>
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="42"/>
-      <c r="D10" s="45" t="s">
+      <c r="C10" s="49"/>
+      <c r="D10" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="37" t="s">
         <v>66</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="32"/>
-      <c r="H10" s="52"/>
+      <c r="H10" s="47"/>
       <c r="L10" s="20" t="s">
         <v>38</v>
       </c>
@@ -1573,11 +1571,11 @@
       </c>
     </row>
     <row r="11" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="44"/>
-      <c r="D11" s="53" t="s">
+      <c r="C11" s="36"/>
+      <c r="D11" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="41" t="s">
         <v>68</v>
       </c>
       <c r="F11" s="34"/>
@@ -1585,14 +1583,14 @@
         <v>67</v>
       </c>
       <c r="H11" s="33"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="47"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="39"/>
     </row>
     <row r="12" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="15" t="s">
         <v>30</v>
       </c>
@@ -1654,10 +1652,10 @@
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="38"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="26" t="s">
         <v>41</v>
       </c>
@@ -1668,8 +1666,8 @@
       <c r="H16" s="25"/>
     </row>
     <row r="17" spans="3:8" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="37"/>
-      <c r="D17" s="39"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="15" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Improved dayy 3 presentation for younger group
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437357B8-5324-484A-A97D-CED880DF23DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66167704-EA1A-4BB9-AAC0-3B5885841A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="младшая" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
   <si>
     <t>lesson 1</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Игра шпион, надо угадать кто шпион. Есть вопрос на который детйи отвечают, но одному дан только ответ из нейросети.</t>
-  </si>
-  <si>
-    <t>Создание сайта - html + css</t>
   </si>
   <si>
     <t xml:space="preserve">Сравнение языков + подводка к созданию сайта как у больших ИТ компаний </t>
@@ -727,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -886,9 +883,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -899,8 +893,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFAFFFAB"/>
       <color rgb="FFFFB871"/>
-      <color rgb="FFAFFFAB"/>
       <color rgb="FFFFEE6D"/>
       <color rgb="FFFF9393"/>
     </mruColors>
@@ -1181,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,14 +1231,14 @@
         <v>1</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="16"/>
       <c r="L6" s="6"/>
@@ -1261,10 +1255,10 @@
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H7" s="14"/>
       <c r="L7" s="8"/>
@@ -1284,7 +1278,7 @@
         <v>27</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="16"/>
       <c r="L8" s="19"/>
@@ -1296,11 +1290,11 @@
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="31" t="s">
         <v>28</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>65</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -1317,21 +1311,21 @@
         <v>10</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10" s="16"/>
       <c r="L10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="21" t="s">
         <v>38</v>
-      </c>
-      <c r="M10" s="21" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1339,10 +1333,10 @@
         <v>11</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -1353,14 +1347,14 @@
         <v>12</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="16"/>
     </row>
@@ -1369,10 +1363,10 @@
         <v>13</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
@@ -1384,11 +1378,11 @@
       </c>
       <c r="D14" s="44"/>
       <c r="E14" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="24"/>
       <c r="G14" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H14" s="25"/>
     </row>
@@ -1396,13 +1390,13 @@
       <c r="C15" s="43"/>
       <c r="D15" s="45"/>
       <c r="E15" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H15" s="16"/>
     </row>
@@ -1422,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53492BD-B09C-4A09-8913-63C13D46C685}">
   <dimension ref="C3:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,14 +1453,14 @@
         <v>0</v>
       </c>
       <c r="D5" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>58</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>59</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="14"/>
       <c r="L5" s="4"/>
@@ -1486,7 +1480,7 @@
         <v>22</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="16"/>
       <c r="L6" s="6"/>
@@ -1499,14 +1493,14 @@
         <v>7</v>
       </c>
       <c r="D7" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="31" t="s">
         <v>60</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>61</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" s="14"/>
       <c r="L7" s="8"/>
@@ -1526,7 +1520,7 @@
         <v>27</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="16"/>
       <c r="L8" s="19"/>
@@ -1539,7 +1533,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="40"/>
       <c r="F9" s="50"/>
@@ -1555,32 +1549,32 @@
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="49"/>
       <c r="D10" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="32"/>
       <c r="H10" s="47"/>
       <c r="L10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="21" t="s">
         <v>38</v>
-      </c>
-      <c r="M10" s="21" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C11" s="36"/>
       <c r="D11" s="52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="33"/>
       <c r="L11" s="38"/>
@@ -1592,15 +1586,15 @@
       </c>
       <c r="D12" s="53"/>
       <c r="E12" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="16"/>
       <c r="M12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1608,14 +1602,14 @@
         <v>11</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -1624,14 +1618,14 @@
         <v>12</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H14" s="16"/>
     </row>
@@ -1640,14 +1634,14 @@
         <v>13</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -1657,11 +1651,11 @@
       </c>
       <c r="D16" s="44"/>
       <c r="E16" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="24"/>
       <c r="G16" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H16" s="25"/>
     </row>
@@ -1669,13 +1663,13 @@
       <c r="C17" s="43"/>
       <c r="D17" s="45"/>
       <c r="E17" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H17" s="16"/>
     </row>

</xml_diff>

<commit_message>
Added day 1 presentation for younger group
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66167704-EA1A-4BB9-AAC0-3B5885841A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB85ADAB-894A-4799-8168-B71EC03E0857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="младшая" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
   <si>
     <t>lesson 1</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>Создания сайта с помощью нейросети, neocities.org</t>
+  </si>
+  <si>
+    <t>zadanije</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,12 +365,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -724,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -808,12 +805,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -895,8 +886,8 @@
     <mruColors>
       <color rgb="FFAFFFAB"/>
       <color rgb="FFFFB871"/>
+      <color rgb="FFFF9393"/>
       <color rgb="FFFFEE6D"/>
-      <color rgb="FFFF9393"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1175,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,11 +1203,13 @@
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="13"/>
@@ -1254,10 +1247,10 @@
         <v>23</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="13" t="s">
         <v>48</v>
       </c>
       <c r="H7" s="14"/>
@@ -1274,7 +1267,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="33" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="15" t="s">
@@ -1290,10 +1283,10 @@
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="29" t="s">
         <v>65</v>
       </c>
       <c r="F9" s="13"/>
@@ -1310,7 +1303,7 @@
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="33" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="15" t="s">
@@ -1373,10 +1366,10 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="44"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="26" t="s">
         <v>40</v>
       </c>
@@ -1387,8 +1380,8 @@
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="43"/>
-      <c r="D15" s="45"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="43"/>
       <c r="E15" s="15" t="s">
         <v>41</v>
       </c>
@@ -1416,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53492BD-B09C-4A09-8913-63C13D46C685}">
   <dimension ref="C3:M18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,14 +1445,14 @@
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="29" t="s">
         <v>58</v>
       </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="29" t="s">
         <v>61</v>
       </c>
       <c r="H5" s="14"/>
@@ -1492,14 +1485,14 @@
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="29" t="s">
         <v>60</v>
       </c>
       <c r="F7" s="13"/>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="29" t="s">
         <v>61</v>
       </c>
       <c r="H7" s="14"/>
@@ -1516,7 +1509,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="33" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="15" t="s">
@@ -1529,16 +1522,16 @@
       </c>
     </row>
     <row r="9" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="46"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="44"/>
       <c r="L9" s="22" t="s">
         <v>24</v>
       </c>
@@ -1547,16 +1540,16 @@
       </c>
     </row>
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="49"/>
-      <c r="D10" s="37" t="s">
+      <c r="C10" s="47"/>
+      <c r="D10" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="51"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="47"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="45"/>
       <c r="L10" s="20" t="s">
         <v>37</v>
       </c>
@@ -1565,26 +1558,26 @@
       </c>
     </row>
     <row r="11" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="36"/>
-      <c r="D11" s="52" t="s">
+      <c r="C11" s="34"/>
+      <c r="D11" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="34"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="33"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="39"/>
+      <c r="H11" s="31"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="37"/>
     </row>
     <row r="12" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="53"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="15" t="s">
         <v>29</v>
       </c>
@@ -1646,10 +1639,10 @@
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="44"/>
+      <c r="D16" s="42"/>
       <c r="E16" s="26" t="s">
         <v>40</v>
       </c>
@@ -1660,8 +1653,8 @@
       <c r="H16" s="25"/>
     </row>
     <row r="17" spans="3:8" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="43"/>
-      <c r="D17" s="45"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="43"/>
       <c r="E17" s="15" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Added day 4 unity presentation
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB85ADAB-894A-4799-8168-B71EC03E0857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CFE768-B783-4874-91B0-86EAB0ED91C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -721,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -874,6 +874,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1167,7 +1170,7 @@
   <dimension ref="C3:M16"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53492BD-B09C-4A09-8913-63C13D46C685}">
   <dimension ref="C3:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,14 +1597,14 @@
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="52" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="17"/>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="52" t="s">
         <v>50</v>
       </c>
       <c r="H13" s="18"/>

</xml_diff>

<commit_message>
Changed/Added day 2, 4 presentations
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CFE768-B783-4874-91B0-86EAB0ED91C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7B2044-5E07-4D81-BF9F-EF755B7CDB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,28 @@
     <sheet name="младшая" sheetId="1" r:id="rId1"/>
     <sheet name="старшая" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
   <si>
     <t>lesson 1</t>
   </si>
@@ -89,9 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve">Игра в сломанный телефон на морском коде </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Первый и - советник императора </t>
   </si>
   <si>
     <t xml:space="preserve">Игра в стратегию где дети разделяются по парам - советник и император </t>
@@ -231,12 +239,6 @@
     <t>Презентация о unity и подводка к заданию - надо представить как будет выглядеть  город в будущем</t>
   </si>
   <si>
-    <t>Исправляют баг в коде с комментариями + github</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сингулярность + про далекое будущее + базовые команды для управления роботом в майнкрафт </t>
-  </si>
-  <si>
     <t>Сингулярность + про далекое будущее</t>
   </si>
   <si>
@@ -279,7 +281,16 @@
     <t>Создания сайта с помощью нейросети, neocities.org</t>
   </si>
   <si>
-    <t>zadanije</t>
+    <t>Исправляют баг в коде с комментариями</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Базовые команды для управления роботом в майнкрафт </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Появление ии - немного истории </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + python jesli budetj vremja</t>
   </si>
 </sst>
 </file>
@@ -721,7 +732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -804,9 +815,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -840,6 +848,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -874,9 +885,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1167,9 +1175,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:M16"/>
+  <dimension ref="C3:M17"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1206,13 +1214,11 @@
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="13"/>
@@ -1227,14 +1233,14 @@
         <v>1</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" s="16"/>
       <c r="L6" s="6"/>
@@ -1246,17 +1252,19 @@
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>23</v>
+      <c r="D7" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="14"/>
+      <c r="F7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>68</v>
+      </c>
       <c r="L7" s="8"/>
       <c r="M7" s="7" t="s">
         <v>17</v>
@@ -1266,15 +1274,15 @@
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="33" t="s">
-        <v>27</v>
-      </c>
       <c r="G8" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="16"/>
       <c r="L8" s="19"/>
@@ -1286,53 +1294,53 @@
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>65</v>
+      <c r="D9" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>62</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="14"/>
       <c r="L9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="23" t="s">
         <v>24</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="33" t="s">
-        <v>30</v>
+      <c r="D10" s="32" t="s">
+        <v>29</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H10" s="16"/>
       <c r="L10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="21" t="s">
         <v>37</v>
-      </c>
-      <c r="M10" s="21" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="13" t="s">
+      <c r="D11" s="28" t="s">
         <v>31</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -1342,65 +1350,75 @@
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15" t="s">
+      <c r="G12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+      <c r="D13" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="40" t="s">
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="3:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="26" t="s">
+      <c r="D15" s="42"/>
+      <c r="E15" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="41"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24" t="s">
+      <c r="F16" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="41"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="16"/>
-    </row>
-    <row r="16" spans="3:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1412,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53492BD-B09C-4A09-8913-63C13D46C685}">
   <dimension ref="C3:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,15 +1466,15 @@
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="29" t="s">
+      <c r="D5" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="28" t="s">
         <v>58</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="29" t="s">
-        <v>61</v>
       </c>
       <c r="H5" s="14"/>
       <c r="L5" s="4"/>
@@ -1469,14 +1487,14 @@
         <v>1</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" s="16"/>
       <c r="L6" s="6"/>
@@ -1488,15 +1506,15 @@
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>60</v>
+      <c r="D7" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="F7" s="13"/>
-      <c r="G7" s="29" t="s">
-        <v>61</v>
+      <c r="G7" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H7" s="14"/>
       <c r="L7" s="8"/>
@@ -1508,15 +1526,15 @@
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="33" t="s">
-        <v>27</v>
-      </c>
       <c r="G8" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="16"/>
       <c r="L8" s="19"/>
@@ -1528,53 +1546,53 @@
       <c r="C9" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="38"/>
+      <c r="D9" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="37"/>
       <c r="F9" s="48"/>
-      <c r="G9" s="38"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="44"/>
       <c r="L9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="23" t="s">
         <v>24</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="47"/>
-      <c r="D10" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>65</v>
+      <c r="D10" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="F10" s="49"/>
-      <c r="G10" s="30"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="45"/>
       <c r="L10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="M10" s="21" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="11" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="34"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="32"/>
+        <v>29</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="31"/>
       <c r="G11" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="31"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
+        <v>63</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="36"/>
     </row>
     <row r="12" spans="3:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
@@ -1582,30 +1600,30 @@
       </c>
       <c r="D12" s="51"/>
       <c r="E12" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="16"/>
       <c r="M12" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="3:13" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="52" t="s">
+      <c r="D13" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="39" t="s">
         <v>49</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="52" t="s">
-        <v>50</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -1613,15 +1631,15 @@
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15" t="s">
-        <v>34</v>
-      </c>
       <c r="G14" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H14" s="16"/>
     </row>
@@ -1629,15 +1647,15 @@
       <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="D15" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="39" t="s">
         <v>52</v>
-      </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17" t="s">
-        <v>55</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -1647,11 +1665,11 @@
       </c>
       <c r="D16" s="42"/>
       <c r="E16" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="24"/>
       <c r="G16" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H16" s="25"/>
     </row>
@@ -1659,13 +1677,13 @@
       <c r="C17" s="41"/>
       <c r="D17" s="43"/>
       <c r="E17" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H17" s="16"/>
     </row>

</xml_diff>

<commit_message>
day 5 minecraft map + presentation
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troks\Desktop\HelloIt\HelloIT_campl_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7B2044-5E07-4D81-BF9F-EF755B7CDB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC038768-0771-4B1E-8A37-9DE3FD1F4955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -896,9 +896,9 @@
   <colors>
     <mruColors>
       <color rgb="FFAFFFAB"/>
+      <color rgb="FFFFEE6D"/>
       <color rgb="FFFFB871"/>
       <color rgb="FFFF9393"/>
-      <color rgb="FFFFEE6D"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1177,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,10 +1376,10 @@
       <c r="C14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="39" t="s">
         <v>34</v>
       </c>
       <c r="F14" s="17"/>
@@ -1431,7 +1431,7 @@
   <dimension ref="C3:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>